<commit_message>
add provider and medicine columns to spreadsheet, remove event providers
</commit_message>
<xml_diff>
--- a/app/data/base_export.xlsx
+++ b/app/data/base_export.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="55">
   <si>
     <t>Camp</t>
   </si>
@@ -46,6 +46,9 @@
     <t>Phone</t>
   </si>
   <si>
+    <t>Provider</t>
+  </si>
+  <si>
     <t>Medical Hx</t>
   </si>
   <si>
@@ -76,9 +79,6 @@
     <t>Deprecated Fields</t>
   </si>
   <si>
-    <t>Medical Provider</t>
-  </si>
-  <si>
     <t>Allergies</t>
   </si>
   <si>
@@ -146,6 +146,12 @@
   </si>
   <si>
     <t>Medication 3</t>
+  </si>
+  <si>
+    <t>Medication 4</t>
+  </si>
+  <si>
+    <t>Medication 5</t>
   </si>
   <si>
     <t>Previous Treatment</t>
@@ -233,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -251,6 +257,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
@@ -272,6 +281,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -498,41 +510,38 @@
     <col customWidth="1" min="3" max="3" width="11.78"/>
     <col customWidth="1" min="4" max="8" width="10.56"/>
     <col customWidth="1" min="9" max="9" width="12.67"/>
-    <col customWidth="1" min="10" max="11" width="10.56"/>
-    <col customWidth="1" min="12" max="12" width="14.89"/>
-    <col customWidth="1" min="13" max="14" width="10.56"/>
+    <col customWidth="1" min="10" max="12" width="10.56"/>
+    <col customWidth="1" min="13" max="13" width="14.11"/>
+    <col customWidth="1" min="14" max="14" width="10.56"/>
     <col customWidth="1" min="15" max="15" width="16.33"/>
     <col customWidth="1" min="16" max="17" width="10.56"/>
-    <col customWidth="1" min="18" max="19" width="15.44"/>
-    <col customWidth="1" min="20" max="26" width="10.56"/>
-    <col customWidth="1" min="27" max="27" width="21.0"/>
-    <col customWidth="1" min="28" max="28" width="15.11"/>
-    <col customWidth="1" min="29" max="29" width="18.89"/>
-    <col customWidth="1" min="30" max="30" width="14.89"/>
-    <col customWidth="1" min="31" max="31" width="15.56"/>
-    <col customWidth="1" min="32" max="32" width="17.89"/>
-    <col customWidth="1" min="33" max="33" width="17.11"/>
-    <col customWidth="1" min="34" max="41" width="13.33"/>
-    <col customWidth="1" min="42" max="42" width="14.11"/>
-    <col customWidth="1" min="43" max="43" width="12.44"/>
-    <col customWidth="1" min="44" max="44" width="14.0"/>
-    <col customWidth="1" min="45" max="47" width="11.67"/>
-    <col customWidth="1" min="48" max="48" width="12.44"/>
-    <col customWidth="1" min="49" max="49" width="15.78"/>
-    <col customWidth="1" min="50" max="50" width="16.67"/>
-    <col customWidth="1" min="51" max="52" width="10.56"/>
-    <col customWidth="1" min="53" max="53" width="12.44"/>
-    <col customWidth="1" min="54" max="54" width="15.89"/>
-    <col customWidth="1" min="55" max="55" width="15.44"/>
-    <col customWidth="1" min="56" max="56" width="10.56"/>
-    <col customWidth="1" min="57" max="57" width="15.0"/>
-    <col customWidth="1" min="58" max="58" width="15.11"/>
-    <col customWidth="1" min="59" max="59" width="10.56"/>
-    <col customWidth="1" min="60" max="60" width="17.67"/>
-    <col customWidth="1" min="61" max="61" width="14.11"/>
-    <col customWidth="1" min="62" max="63" width="10.56"/>
-    <col customWidth="1" min="64" max="64" width="18.89"/>
-    <col customWidth="1" min="65" max="67" width="10.56"/>
+    <col customWidth="1" min="18" max="18" width="15.44"/>
+    <col customWidth="1" min="19" max="25" width="10.56"/>
+    <col customWidth="1" min="26" max="26" width="15.11"/>
+    <col customWidth="1" min="27" max="27" width="18.89"/>
+    <col customWidth="1" min="28" max="28" width="14.89"/>
+    <col customWidth="1" min="29" max="29" width="15.56"/>
+    <col customWidth="1" min="30" max="30" width="17.89"/>
+    <col customWidth="1" min="31" max="31" width="17.11"/>
+    <col customWidth="1" min="32" max="37" width="13.33"/>
+    <col customWidth="1" min="38" max="38" width="14.11"/>
+    <col customWidth="1" min="39" max="39" width="12.44"/>
+    <col customWidth="1" min="40" max="42" width="11.67"/>
+    <col customWidth="1" min="43" max="51" width="12.44"/>
+    <col customWidth="1" min="52" max="52" width="16.67"/>
+    <col customWidth="1" min="53" max="54" width="10.56"/>
+    <col customWidth="1" min="55" max="55" width="12.44"/>
+    <col customWidth="1" min="56" max="56" width="15.89"/>
+    <col customWidth="1" min="57" max="57" width="15.44"/>
+    <col customWidth="1" min="58" max="58" width="10.56"/>
+    <col customWidth="1" min="59" max="59" width="15.0"/>
+    <col customWidth="1" min="60" max="60" width="15.11"/>
+    <col customWidth="1" min="61" max="61" width="10.56"/>
+    <col customWidth="1" min="62" max="62" width="17.67"/>
+    <col customWidth="1" min="63" max="63" width="14.11"/>
+    <col customWidth="1" min="64" max="65" width="10.56"/>
+    <col customWidth="1" min="66" max="66" width="18.89"/>
+    <col customWidth="1" min="67" max="69" width="10.56"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -569,19 +578,21 @@
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5"/>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
       <c r="R1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="S1" s="5" t="s">
         <v>13</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="T1" s="5"/>
       <c r="U1" s="5"/>
@@ -589,19 +600,19 @@
       <c r="W1" s="5"/>
       <c r="X1" s="5"/>
       <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="Z1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
       <c r="AE1" s="1"/>
-      <c r="AF1" s="1"/>
+      <c r="AF1" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="AG1" s="1"/>
-      <c r="AH1" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="AH1" s="1"/>
       <c r="AI1" s="1"/>
       <c r="AJ1" s="1"/>
       <c r="AK1" s="1"/>
@@ -616,1114 +627,1117 @@
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
-      <c r="AW1" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="AW1" s="1"/>
       <c r="AX1" s="1"/>
       <c r="AY1" s="1"/>
-      <c r="AZ1" s="1"/>
+      <c r="AZ1" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="BA1" s="1"/>
       <c r="BB1" s="1"/>
       <c r="BC1" s="1"/>
       <c r="BD1" s="1"/>
-      <c r="BE1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="BF1" s="2" t="s">
+      <c r="BE1" s="1"/>
+      <c r="BF1" s="1"/>
+      <c r="BG1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="BG1" s="5" t="s">
+      <c r="BH1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="BH1" s="6" t="s">
+      <c r="BI1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="BI1" s="7"/>
-      <c r="BJ1" s="7"/>
-      <c r="BK1" s="7"/>
-      <c r="BL1" s="7"/>
-      <c r="BM1" s="7"/>
-      <c r="BN1" s="7"/>
-      <c r="BO1" s="7"/>
+      <c r="BJ1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BK1" s="8"/>
+      <c r="BL1" s="8"/>
+      <c r="BM1" s="8"/>
+      <c r="BN1" s="8"/>
+      <c r="BO1" s="8"/>
+      <c r="BP1" s="8"/>
+      <c r="BQ1" s="8"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" s="10" t="s">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="N2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="O2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="10" t="s">
+      <c r="P2" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="Q2" s="10" t="s">
+      <c r="Q2" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="R2" s="11"/>
-      <c r="S2" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="T2" s="12" t="s">
+      <c r="R2" s="12"/>
+      <c r="S2" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="U2" s="12" t="s">
+      <c r="T2" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="V2" s="12" t="s">
+      <c r="U2" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="W2" s="10" t="s">
+      <c r="V2" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="X2" s="10" t="s">
+      <c r="W2" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="Y2" s="10" t="s">
+      <c r="X2" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="Z2" s="12" t="s">
+      <c r="Y2" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="AA2" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="AB2" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC2" s="10" t="s">
+      <c r="Z2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA2" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="AD2" s="10" t="s">
+      <c r="AB2" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="AE2" s="10" t="s">
+      <c r="AC2" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="AF2" s="10" t="s">
+      <c r="AD2" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="AG2" s="10" t="s">
+      <c r="AE2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="AH2" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="AI2" s="10" t="s">
+      <c r="AF2" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="AJ2" s="10" t="s">
+      <c r="AG2" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="AK2" s="10" t="s">
+      <c r="AH2" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="AL2" s="10" t="s">
+      <c r="AI2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="AM2" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="AN2" s="10" t="s">
+      <c r="AJ2" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="AO2" s="10" t="s">
+      <c r="AK2" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="AP2" s="10" t="s">
+      <c r="AL2" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="AQ2" s="10" t="s">
+      <c r="AM2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="AR2" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="AS2" s="10" t="s">
+      <c r="AN2" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="AT2" s="10" t="s">
+      <c r="AO2" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="AU2" s="10" t="s">
+      <c r="AP2" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="AV2" s="10" t="s">
+      <c r="AQ2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="AW2" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="AX2" s="10" t="s">
+      <c r="AR2" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="AY2" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AZ2" s="10" t="s">
+      <c r="AS2" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="AT2" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="AU2" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="AV2" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="BA2" s="10" t="s">
+      <c r="AW2" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="AX2" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="AY2" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="AZ2" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="BB2" s="10" t="s">
+      <c r="BA2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="BB2" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="BC2" s="10" t="s">
+      <c r="BC2" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="BD2" s="10" t="s">
+      <c r="BD2" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="BE2" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="BF2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="BE2" s="8"/>
-      <c r="BF2" s="8"/>
-      <c r="BG2" s="8"/>
-      <c r="BH2" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="BI2" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="BJ2" s="13" t="s">
+      <c r="BG2" s="9"/>
+      <c r="BH2" s="9"/>
+      <c r="BI2" s="9"/>
+      <c r="BJ2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="BK2" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="BL2" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="BK2" s="13" t="s">
+      <c r="BM2" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="BL2" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="BM2" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="BN2" s="13" t="s">
+      <c r="BN2" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="BO2" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="BP2" s="15" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="14"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
-      <c r="U3" s="14"/>
-      <c r="V3" s="14"/>
-      <c r="W3" s="14"/>
-      <c r="X3" s="14"/>
-      <c r="Y3" s="14"/>
-      <c r="Z3" s="14"/>
-      <c r="AA3" s="14"/>
-      <c r="AB3" s="14"/>
-      <c r="AC3" s="14"/>
-      <c r="AD3" s="14"/>
-      <c r="AE3" s="14"/>
-      <c r="AF3" s="14"/>
-      <c r="AG3" s="14"/>
-      <c r="AH3" s="14"/>
-      <c r="AI3" s="14"/>
-      <c r="AJ3" s="14"/>
-      <c r="AK3" s="14"/>
-      <c r="AL3" s="14"/>
-      <c r="AM3" s="14"/>
-      <c r="AN3" s="14"/>
-      <c r="AO3" s="14"/>
-      <c r="AP3" s="14"/>
-      <c r="AQ3" s="14"/>
-      <c r="AR3" s="14"/>
-      <c r="AS3" s="14"/>
-      <c r="AT3" s="14"/>
-      <c r="AU3" s="14"/>
-      <c r="AV3" s="14"/>
-      <c r="AW3" s="14"/>
-      <c r="AX3" s="14"/>
-      <c r="AY3" s="14"/>
-      <c r="AZ3" s="14"/>
-      <c r="BA3" s="14"/>
-      <c r="BB3" s="14"/>
-      <c r="BC3" s="14"/>
-      <c r="BD3" s="14"/>
-      <c r="BE3" s="14"/>
-      <c r="BF3" s="14"/>
-      <c r="BG3" s="14"/>
-      <c r="BH3" s="14"/>
-      <c r="BI3" s="14"/>
-      <c r="BJ3" s="14"/>
-      <c r="BK3" s="14"/>
-      <c r="BL3" s="14"/>
-      <c r="BM3" s="14"/>
-      <c r="BN3" s="14"/>
-      <c r="BO3" s="14"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="16"/>
+      <c r="T3" s="16"/>
+      <c r="U3" s="16"/>
+      <c r="V3" s="16"/>
+      <c r="W3" s="16"/>
+      <c r="X3" s="16"/>
+      <c r="Y3" s="16"/>
+      <c r="Z3" s="16"/>
+      <c r="AA3" s="16"/>
+      <c r="AB3" s="16"/>
+      <c r="AC3" s="16"/>
+      <c r="AD3" s="16"/>
+      <c r="AE3" s="16"/>
+      <c r="AF3" s="16"/>
+      <c r="AG3" s="16"/>
+      <c r="AH3" s="16"/>
+      <c r="AI3" s="16"/>
+      <c r="AJ3" s="16"/>
+      <c r="AK3" s="16"/>
+      <c r="AL3" s="16"/>
+      <c r="AM3" s="16"/>
+      <c r="AN3" s="16"/>
+      <c r="AO3" s="16"/>
+      <c r="AP3" s="16"/>
+      <c r="AQ3" s="16"/>
+      <c r="AR3" s="16"/>
+      <c r="AS3" s="16"/>
+      <c r="AT3" s="16"/>
+      <c r="AU3" s="16"/>
+      <c r="AV3" s="16"/>
+      <c r="AW3" s="16"/>
+      <c r="AX3" s="16"/>
+      <c r="AY3" s="16"/>
+      <c r="AZ3" s="16"/>
+      <c r="BA3" s="16"/>
+      <c r="BB3" s="16"/>
+      <c r="BC3" s="16"/>
+      <c r="BD3" s="16"/>
+      <c r="BE3" s="16"/>
+      <c r="BF3" s="16"/>
+      <c r="BG3" s="16"/>
+      <c r="BH3" s="16"/>
+      <c r="BI3" s="16"/>
+      <c r="BJ3" s="16"/>
+      <c r="BK3" s="16"/>
+      <c r="BL3" s="16"/>
+      <c r="BM3" s="16"/>
+      <c r="BN3" s="16"/>
+      <c r="BO3" s="16"/>
+      <c r="BP3" s="16"/>
+      <c r="BQ3" s="16"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="14"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="14"/>
-      <c r="T4" s="14"/>
-      <c r="U4" s="14"/>
-      <c r="V4" s="14"/>
-      <c r="W4" s="14"/>
-      <c r="X4" s="14"/>
-      <c r="Y4" s="14"/>
-      <c r="Z4" s="14"/>
-      <c r="AA4" s="14"/>
-      <c r="AB4" s="14"/>
-      <c r="AC4" s="14"/>
-      <c r="AD4" s="14"/>
-      <c r="AE4" s="14"/>
-      <c r="AF4" s="14"/>
-      <c r="AG4" s="14"/>
-      <c r="AH4" s="14"/>
-      <c r="AI4" s="14"/>
-      <c r="AJ4" s="14"/>
-      <c r="AK4" s="14"/>
-      <c r="AL4" s="14"/>
-      <c r="AM4" s="14"/>
-      <c r="AN4" s="14"/>
-      <c r="AO4" s="14"/>
-      <c r="AP4" s="14"/>
-      <c r="AQ4" s="14"/>
-      <c r="AR4" s="14"/>
-      <c r="AS4" s="14"/>
-      <c r="AT4" s="14"/>
-      <c r="AU4" s="14"/>
-      <c r="AV4" s="14"/>
-      <c r="AW4" s="14"/>
-      <c r="AX4" s="14"/>
-      <c r="AY4" s="14"/>
-      <c r="AZ4" s="14"/>
-      <c r="BA4" s="14"/>
-      <c r="BB4" s="14"/>
-      <c r="BC4" s="14"/>
-      <c r="BD4" s="14"/>
-      <c r="BE4" s="14"/>
-      <c r="BF4" s="14"/>
-      <c r="BG4" s="14"/>
-      <c r="BH4" s="14"/>
-      <c r="BI4" s="14"/>
-      <c r="BJ4" s="14"/>
-      <c r="BK4" s="14"/>
-      <c r="BL4" s="14"/>
-      <c r="BM4" s="14"/>
-      <c r="BN4" s="14"/>
-      <c r="BO4" s="14"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="16"/>
+      <c r="Y4" s="16"/>
+      <c r="Z4" s="16"/>
+      <c r="AA4" s="16"/>
+      <c r="AB4" s="16"/>
+      <c r="AC4" s="16"/>
+      <c r="AD4" s="16"/>
+      <c r="AE4" s="16"/>
+      <c r="AF4" s="16"/>
+      <c r="AG4" s="16"/>
+      <c r="AH4" s="16"/>
+      <c r="AI4" s="16"/>
+      <c r="AJ4" s="16"/>
+      <c r="AK4" s="16"/>
+      <c r="AL4" s="16"/>
+      <c r="AM4" s="16"/>
+      <c r="AN4" s="16"/>
+      <c r="AO4" s="16"/>
+      <c r="AP4" s="16"/>
+      <c r="AQ4" s="16"/>
+      <c r="AR4" s="16"/>
+      <c r="AS4" s="16"/>
+      <c r="AT4" s="16"/>
+      <c r="AU4" s="16"/>
+      <c r="AV4" s="16"/>
+      <c r="AW4" s="16"/>
+      <c r="AX4" s="16"/>
+      <c r="AY4" s="16"/>
+      <c r="AZ4" s="16"/>
+      <c r="BA4" s="16"/>
+      <c r="BB4" s="16"/>
+      <c r="BC4" s="16"/>
+      <c r="BD4" s="16"/>
+      <c r="BE4" s="16"/>
+      <c r="BF4" s="16"/>
+      <c r="BG4" s="16"/>
+      <c r="BH4" s="16"/>
+      <c r="BI4" s="16"/>
+      <c r="BJ4" s="16"/>
+      <c r="BK4" s="16"/>
+      <c r="BL4" s="16"/>
+      <c r="BM4" s="16"/>
+      <c r="BN4" s="16"/>
+      <c r="BO4" s="16"/>
+      <c r="BP4" s="16"/>
+      <c r="BQ4" s="16"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="14"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14"/>
-      <c r="S5" s="14"/>
-      <c r="T5" s="14"/>
-      <c r="U5" s="14"/>
-      <c r="V5" s="14"/>
-      <c r="W5" s="14"/>
-      <c r="X5" s="14"/>
-      <c r="Y5" s="14"/>
-      <c r="Z5" s="14"/>
-      <c r="AA5" s="14"/>
-      <c r="AB5" s="14"/>
-      <c r="AC5" s="14"/>
-      <c r="AD5" s="14"/>
-      <c r="AE5" s="14"/>
-      <c r="AF5" s="14"/>
-      <c r="AG5" s="14"/>
-      <c r="AH5" s="14"/>
-      <c r="AI5" s="14"/>
-      <c r="AJ5" s="14"/>
-      <c r="AK5" s="14"/>
-      <c r="AL5" s="14"/>
-      <c r="AM5" s="14"/>
-      <c r="AN5" s="14"/>
-      <c r="AO5" s="14"/>
-      <c r="AP5" s="14"/>
-      <c r="AQ5" s="14"/>
-      <c r="AR5" s="14"/>
-      <c r="AS5" s="14"/>
-      <c r="AT5" s="14"/>
-      <c r="AU5" s="14"/>
-      <c r="AV5" s="14"/>
-      <c r="AW5" s="14"/>
-      <c r="AX5" s="14"/>
-      <c r="AY5" s="14"/>
-      <c r="AZ5" s="14"/>
-      <c r="BA5" s="14"/>
-      <c r="BB5" s="14"/>
-      <c r="BC5" s="14"/>
-      <c r="BD5" s="14"/>
-      <c r="BE5" s="14"/>
-      <c r="BF5" s="14"/>
-      <c r="BG5" s="14"/>
-      <c r="BH5" s="14"/>
-      <c r="BI5" s="14"/>
-      <c r="BJ5" s="14"/>
-      <c r="BK5" s="14"/>
-      <c r="BL5" s="14"/>
-      <c r="BM5" s="14"/>
-      <c r="BN5" s="14"/>
-      <c r="BO5" s="14"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="16"/>
+      <c r="V5" s="16"/>
+      <c r="W5" s="16"/>
+      <c r="X5" s="16"/>
+      <c r="Y5" s="16"/>
+      <c r="Z5" s="16"/>
+      <c r="AA5" s="16"/>
+      <c r="AB5" s="16"/>
+      <c r="AC5" s="16"/>
+      <c r="AD5" s="16"/>
+      <c r="AE5" s="16"/>
+      <c r="AF5" s="16"/>
+      <c r="AG5" s="16"/>
+      <c r="AH5" s="16"/>
+      <c r="AI5" s="16"/>
+      <c r="AJ5" s="16"/>
+      <c r="AK5" s="16"/>
+      <c r="AL5" s="16"/>
+      <c r="AM5" s="16"/>
+      <c r="AN5" s="16"/>
+      <c r="AO5" s="16"/>
+      <c r="AP5" s="16"/>
+      <c r="AQ5" s="16"/>
+      <c r="AR5" s="16"/>
+      <c r="AS5" s="16"/>
+      <c r="AT5" s="16"/>
+      <c r="AU5" s="16"/>
+      <c r="AV5" s="16"/>
+      <c r="AW5" s="16"/>
+      <c r="AX5" s="16"/>
+      <c r="AY5" s="16"/>
+      <c r="AZ5" s="16"/>
+      <c r="BA5" s="16"/>
+      <c r="BB5" s="16"/>
+      <c r="BC5" s="16"/>
+      <c r="BD5" s="16"/>
+      <c r="BE5" s="16"/>
+      <c r="BF5" s="16"/>
+      <c r="BG5" s="16"/>
+      <c r="BH5" s="16"/>
+      <c r="BI5" s="16"/>
+      <c r="BJ5" s="16"/>
+      <c r="BK5" s="16"/>
+      <c r="BL5" s="16"/>
+      <c r="BM5" s="16"/>
+      <c r="BN5" s="16"/>
+      <c r="BO5" s="16"/>
+      <c r="BP5" s="16"/>
+      <c r="BQ5" s="16"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="14"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="14"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="X7" s="14"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="W7" s="16"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="14"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="L8" s="14"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="L9" s="14"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="14"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="L10" s="14"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="14"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="L11" s="14"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="14"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="L12" s="14"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="14"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="L13" s="14"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="H13" s="16"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="C14" s="14"/>
+      <c r="C14" s="16"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="C15" s="14"/>
+      <c r="C15" s="16"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="C16" s="14"/>
+      <c r="C16" s="16"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="C17" s="14"/>
+      <c r="C17" s="16"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="C18" s="14"/>
+      <c r="C18" s="16"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="C19" s="14"/>
+      <c r="C19" s="16"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="C20" s="14"/>
+      <c r="C20" s="16"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="C21" s="14"/>
+      <c r="C21" s="16"/>
     </row>
     <row r="22" ht="15.75" customHeight="1"/>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="C23" s="14"/>
+      <c r="C23" s="16"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="C24" s="14"/>
+      <c r="C24" s="16"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="C25" s="14"/>
+      <c r="C25" s="16"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="C26" s="14"/>
+      <c r="C26" s="16"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="C27" s="14"/>
+      <c r="C27" s="16"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="C28" s="14"/>
+      <c r="C28" s="16"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="C29" s="14"/>
+      <c r="C29" s="16"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="C30" s="14"/>
+      <c r="C30" s="16"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="C31" s="14"/>
+      <c r="C31" s="16"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="C32" s="14"/>
+      <c r="C32" s="16"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="C33" s="14"/>
+      <c r="C33" s="16"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="C34" s="14"/>
+      <c r="C34" s="16"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="C35" s="14"/>
+      <c r="C35" s="16"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="C36" s="14"/>
+      <c r="C36" s="16"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="C37" s="14"/>
+      <c r="C37" s="16"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="C38" s="14"/>
+      <c r="C38" s="16"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="C39" s="14"/>
+      <c r="C39" s="16"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="C40" s="14"/>
+      <c r="C40" s="16"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="C41" s="14"/>
+      <c r="C41" s="16"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="C42" s="14"/>
+      <c r="C42" s="16"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="C43" s="14"/>
+      <c r="C43" s="16"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="C44" s="14"/>
+      <c r="C44" s="16"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="C45" s="14"/>
+      <c r="C45" s="16"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="C46" s="14"/>
+      <c r="C46" s="16"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="C47" s="14"/>
+      <c r="C47" s="16"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="C48" s="14"/>
+      <c r="C48" s="16"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="C49" s="14"/>
+      <c r="C49" s="16"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="C50" s="14"/>
+      <c r="C50" s="16"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="C51" s="14"/>
+      <c r="C51" s="16"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="C52" s="14"/>
+      <c r="C52" s="16"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="C53" s="14"/>
+      <c r="C53" s="16"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="C54" s="14"/>
+      <c r="C54" s="16"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="C55" s="14"/>
+      <c r="C55" s="16"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="C56" s="14"/>
+      <c r="C56" s="16"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="C57" s="14"/>
+      <c r="C57" s="16"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="C58" s="14"/>
+      <c r="C58" s="16"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="C59" s="14"/>
+      <c r="C59" s="16"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="C60" s="14"/>
+      <c r="C60" s="16"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="C61" s="14"/>
+      <c r="C61" s="16"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="C62" s="14"/>
+      <c r="C62" s="16"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="C63" s="14"/>
+      <c r="C63" s="16"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="C64" s="14"/>
+      <c r="C64" s="16"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="C65" s="14"/>
+      <c r="C65" s="16"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="C66" s="14"/>
+      <c r="C66" s="16"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="C67" s="14"/>
+      <c r="C67" s="16"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="C68" s="14"/>
+      <c r="C68" s="16"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="C69" s="14"/>
+      <c r="C69" s="16"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="C70" s="14"/>
+      <c r="C70" s="16"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="C71" s="14"/>
+      <c r="C71" s="16"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="C72" s="14"/>
+      <c r="C72" s="16"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="C73" s="14"/>
+      <c r="C73" s="16"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="C74" s="14"/>
+      <c r="C74" s="16"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="C75" s="14"/>
+      <c r="C75" s="16"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="C76" s="14"/>
+      <c r="C76" s="16"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="C77" s="14"/>
+      <c r="C77" s="16"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="C78" s="14"/>
+      <c r="C78" s="16"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="C79" s="14"/>
+      <c r="C79" s="16"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="C80" s="14"/>
+      <c r="C80" s="16"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="C81" s="14"/>
+      <c r="C81" s="16"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="C82" s="14"/>
+      <c r="C82" s="16"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="C83" s="14"/>
+      <c r="C83" s="16"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="C84" s="14"/>
+      <c r="C84" s="16"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="C85" s="14"/>
+      <c r="C85" s="16"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="C86" s="14"/>
+      <c r="C86" s="16"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="C87" s="14"/>
+      <c r="C87" s="16"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="C88" s="14"/>
+      <c r="C88" s="16"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="C89" s="14"/>
+      <c r="C89" s="16"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="C90" s="14"/>
+      <c r="C90" s="16"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="C91" s="14"/>
+      <c r="C91" s="16"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="C92" s="14"/>
+      <c r="C92" s="16"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="C93" s="14"/>
+      <c r="C93" s="16"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="C94" s="14"/>
+      <c r="C94" s="16"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="C95" s="14"/>
+      <c r="C95" s="16"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="C96" s="14"/>
+      <c r="C96" s="16"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="C97" s="14"/>
+      <c r="C97" s="16"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="C98" s="14"/>
+      <c r="C98" s="16"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="C99" s="14"/>
+      <c r="C99" s="16"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="C100" s="14"/>
+      <c r="C100" s="16"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="C101" s="14"/>
+      <c r="C101" s="16"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="C102" s="14"/>
+      <c r="C102" s="16"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="C103" s="14"/>
+      <c r="C103" s="16"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="C104" s="14"/>
+      <c r="C104" s="16"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="C105" s="14"/>
+      <c r="C105" s="16"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="C106" s="14"/>
+      <c r="C106" s="16"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="C107" s="14"/>
+      <c r="C107" s="16"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="C108" s="14"/>
+      <c r="C108" s="16"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="C109" s="14"/>
+      <c r="C109" s="16"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="C110" s="14"/>
+      <c r="C110" s="16"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="C111" s="14"/>
+      <c r="C111" s="16"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="C112" s="14"/>
+      <c r="C112" s="16"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="C113" s="14"/>
+      <c r="C113" s="16"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="C114" s="14"/>
+      <c r="C114" s="16"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="C115" s="14"/>
+      <c r="C115" s="16"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="C116" s="14"/>
+      <c r="C116" s="16"/>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="C117" s="14"/>
+      <c r="C117" s="16"/>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="C118" s="14"/>
+      <c r="C118" s="16"/>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="C119" s="14"/>
+      <c r="C119" s="16"/>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="C120" s="14"/>
+      <c r="C120" s="16"/>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="C121" s="14"/>
+      <c r="C121" s="16"/>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="C122" s="14"/>
+      <c r="C122" s="16"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="C123" s="14"/>
+      <c r="C123" s="16"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="C124" s="14"/>
+      <c r="C124" s="16"/>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="C125" s="14"/>
+      <c r="C125" s="16"/>
     </row>
     <row r="126" ht="15.75" customHeight="1">
-      <c r="C126" s="14"/>
+      <c r="C126" s="16"/>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="C127" s="14"/>
+      <c r="C127" s="16"/>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="C128" s="14"/>
+      <c r="C128" s="16"/>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="C129" s="14"/>
+      <c r="C129" s="16"/>
     </row>
     <row r="130" ht="15.75" customHeight="1">
-      <c r="C130" s="14"/>
+      <c r="C130" s="16"/>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="C131" s="14"/>
+      <c r="C131" s="16"/>
     </row>
     <row r="132" ht="15.75" customHeight="1">
-      <c r="C132" s="14"/>
+      <c r="C132" s="16"/>
     </row>
     <row r="133" ht="15.75" customHeight="1">
-      <c r="C133" s="14"/>
+      <c r="C133" s="16"/>
     </row>
     <row r="134" ht="15.75" customHeight="1">
-      <c r="C134" s="14"/>
+      <c r="C134" s="16"/>
     </row>
     <row r="135" ht="15.75" customHeight="1">
-      <c r="C135" s="14"/>
+      <c r="C135" s="16"/>
     </row>
     <row r="136" ht="15.75" customHeight="1">
-      <c r="C136" s="14"/>
+      <c r="C136" s="16"/>
     </row>
     <row r="137" ht="15.75" customHeight="1">
-      <c r="C137" s="14"/>
+      <c r="C137" s="16"/>
     </row>
     <row r="138" ht="15.75" customHeight="1">
-      <c r="C138" s="14"/>
+      <c r="C138" s="16"/>
     </row>
     <row r="139" ht="15.75" customHeight="1">
-      <c r="C139" s="14"/>
+      <c r="C139" s="16"/>
     </row>
     <row r="140" ht="15.75" customHeight="1">
-      <c r="C140" s="14"/>
+      <c r="C140" s="16"/>
     </row>
     <row r="141" ht="15.75" customHeight="1">
-      <c r="C141" s="14"/>
+      <c r="C141" s="16"/>
     </row>
     <row r="142" ht="15.75" customHeight="1">
-      <c r="C142" s="14"/>
+      <c r="C142" s="16"/>
     </row>
     <row r="143" ht="15.75" customHeight="1">
-      <c r="C143" s="14"/>
+      <c r="C143" s="16"/>
     </row>
     <row r="144" ht="15.75" customHeight="1">
-      <c r="C144" s="14"/>
+      <c r="C144" s="16"/>
     </row>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="C145" s="14"/>
+      <c r="C145" s="16"/>
     </row>
     <row r="146" ht="15.75" customHeight="1">
-      <c r="C146" s="14"/>
+      <c r="C146" s="16"/>
     </row>
     <row r="147" ht="15.75" customHeight="1">
-      <c r="C147" s="14"/>
+      <c r="C147" s="16"/>
     </row>
     <row r="148" ht="15.75" customHeight="1">
-      <c r="C148" s="14"/>
+      <c r="C148" s="16"/>
     </row>
     <row r="149" ht="15.75" customHeight="1">
-      <c r="C149" s="14"/>
+      <c r="C149" s="16"/>
     </row>
     <row r="150" ht="15.75" customHeight="1">
-      <c r="C150" s="14"/>
+      <c r="C150" s="16"/>
     </row>
     <row r="151" ht="15.75" customHeight="1">
-      <c r="C151" s="14"/>
+      <c r="C151" s="16"/>
     </row>
     <row r="152" ht="15.75" customHeight="1">
-      <c r="C152" s="14"/>
+      <c r="C152" s="16"/>
     </row>
     <row r="153" ht="15.75" customHeight="1">
-      <c r="C153" s="14"/>
+      <c r="C153" s="16"/>
     </row>
     <row r="154" ht="15.75" customHeight="1">
-      <c r="C154" s="14"/>
+      <c r="C154" s="16"/>
     </row>
     <row r="155" ht="15.75" customHeight="1">
-      <c r="C155" s="14"/>
+      <c r="C155" s="16"/>
     </row>
     <row r="156" ht="15.75" customHeight="1">
-      <c r="C156" s="14"/>
+      <c r="C156" s="16"/>
     </row>
     <row r="157" ht="15.75" customHeight="1">
-      <c r="C157" s="14"/>
+      <c r="C157" s="16"/>
     </row>
     <row r="158" ht="15.75" customHeight="1">
-      <c r="C158" s="14"/>
+      <c r="C158" s="16"/>
     </row>
     <row r="159" ht="15.75" customHeight="1">
-      <c r="C159" s="14"/>
+      <c r="C159" s="16"/>
     </row>
     <row r="160" ht="15.75" customHeight="1">
-      <c r="C160" s="14"/>
+      <c r="C160" s="16"/>
     </row>
     <row r="161" ht="15.75" customHeight="1">
-      <c r="C161" s="14"/>
+      <c r="C161" s="16"/>
     </row>
     <row r="162" ht="15.75" customHeight="1">
-      <c r="C162" s="14"/>
+      <c r="C162" s="16"/>
     </row>
     <row r="163" ht="15.75" customHeight="1">
-      <c r="C163" s="14"/>
+      <c r="C163" s="16"/>
     </row>
     <row r="164" ht="15.75" customHeight="1">
-      <c r="C164" s="14"/>
+      <c r="C164" s="16"/>
     </row>
     <row r="165" ht="15.75" customHeight="1">
-      <c r="C165" s="14"/>
+      <c r="C165" s="16"/>
     </row>
     <row r="166" ht="15.75" customHeight="1">
-      <c r="C166" s="14"/>
+      <c r="C166" s="16"/>
     </row>
     <row r="167" ht="15.75" customHeight="1">
-      <c r="C167" s="14"/>
+      <c r="C167" s="16"/>
     </row>
     <row r="168" ht="15.75" customHeight="1">
-      <c r="C168" s="14"/>
+      <c r="C168" s="16"/>
     </row>
     <row r="169" ht="15.75" customHeight="1">
-      <c r="C169" s="14"/>
+      <c r="C169" s="16"/>
     </row>
     <row r="170" ht="15.75" customHeight="1">
-      <c r="C170" s="14"/>
+      <c r="C170" s="16"/>
     </row>
     <row r="171" ht="15.75" customHeight="1">
-      <c r="C171" s="14"/>
+      <c r="C171" s="16"/>
     </row>
     <row r="172" ht="15.75" customHeight="1">
-      <c r="C172" s="14"/>
+      <c r="C172" s="16"/>
     </row>
     <row r="173" ht="15.75" customHeight="1">
-      <c r="C173" s="14"/>
+      <c r="C173" s="16"/>
     </row>
     <row r="174" ht="15.75" customHeight="1">
-      <c r="C174" s="14"/>
+      <c r="C174" s="16"/>
     </row>
     <row r="175" ht="15.75" customHeight="1">
-      <c r="C175" s="14"/>
+      <c r="C175" s="16"/>
     </row>
     <row r="176" ht="15.75" customHeight="1">
-      <c r="C176" s="14"/>
+      <c r="C176" s="16"/>
     </row>
     <row r="177" ht="15.75" customHeight="1">
-      <c r="C177" s="14"/>
+      <c r="C177" s="16"/>
     </row>
     <row r="178" ht="15.75" customHeight="1">
-      <c r="C178" s="14"/>
+      <c r="C178" s="16"/>
     </row>
     <row r="179" ht="15.75" customHeight="1">
-      <c r="C179" s="14"/>
+      <c r="C179" s="16"/>
     </row>
     <row r="180" ht="15.75" customHeight="1">
-      <c r="C180" s="14"/>
+      <c r="C180" s="16"/>
     </row>
     <row r="181" ht="15.75" customHeight="1">
-      <c r="C181" s="14"/>
+      <c r="C181" s="16"/>
     </row>
     <row r="182" ht="15.75" customHeight="1">
-      <c r="C182" s="14"/>
+      <c r="C182" s="16"/>
     </row>
     <row r="183" ht="15.75" customHeight="1">
-      <c r="C183" s="14"/>
+      <c r="C183" s="16"/>
     </row>
     <row r="184" ht="15.75" customHeight="1">
-      <c r="C184" s="14"/>
+      <c r="C184" s="16"/>
     </row>
     <row r="185" ht="15.75" customHeight="1">
-      <c r="C185" s="14"/>
+      <c r="C185" s="16"/>
     </row>
     <row r="186" ht="15.75" customHeight="1">
-      <c r="C186" s="14"/>
+      <c r="C186" s="16"/>
     </row>
     <row r="187" ht="15.75" customHeight="1">
-      <c r="C187" s="14"/>
+      <c r="C187" s="16"/>
     </row>
     <row r="188" ht="15.75" customHeight="1">
-      <c r="C188" s="14"/>
+      <c r="C188" s="16"/>
     </row>
     <row r="189" ht="15.75" customHeight="1">
-      <c r="C189" s="14"/>
+      <c r="C189" s="16"/>
     </row>
     <row r="190" ht="15.75" customHeight="1">
-      <c r="C190" s="14"/>
+      <c r="C190" s="16"/>
     </row>
     <row r="191" ht="15.75" customHeight="1">
-      <c r="C191" s="14"/>
+      <c r="C191" s="16"/>
     </row>
     <row r="192" ht="15.75" customHeight="1">
-      <c r="C192" s="14"/>
+      <c r="C192" s="16"/>
     </row>
     <row r="193" ht="15.75" customHeight="1">
-      <c r="C193" s="14"/>
+      <c r="C193" s="16"/>
     </row>
     <row r="194" ht="15.75" customHeight="1">
-      <c r="C194" s="14"/>
+      <c r="C194" s="16"/>
     </row>
     <row r="195" ht="15.75" customHeight="1">
-      <c r="C195" s="14"/>
+      <c r="C195" s="16"/>
     </row>
     <row r="196" ht="15.75" customHeight="1">
-      <c r="C196" s="14"/>
+      <c r="C196" s="16"/>
     </row>
     <row r="197" ht="15.75" customHeight="1">
-      <c r="C197" s="14"/>
+      <c r="C197" s="16"/>
     </row>
     <row r="198" ht="15.75" customHeight="1">
-      <c r="C198" s="14"/>
+      <c r="C198" s="16"/>
     </row>
     <row r="199" ht="15.75" customHeight="1">
-      <c r="C199" s="14"/>
+      <c r="C199" s="16"/>
     </row>
     <row r="200" ht="15.75" customHeight="1">
-      <c r="C200" s="14"/>
+      <c r="C200" s="16"/>
     </row>
     <row r="201" ht="15.75" customHeight="1">
-      <c r="C201" s="14"/>
+      <c r="C201" s="16"/>
     </row>
     <row r="202" ht="15.75" customHeight="1">
-      <c r="C202" s="14"/>
+      <c r="C202" s="16"/>
     </row>
     <row r="203" ht="15.75" customHeight="1">
-      <c r="C203" s="14"/>
+      <c r="C203" s="16"/>
     </row>
     <row r="204" ht="15.75" customHeight="1">
-      <c r="C204" s="14"/>
+      <c r="C204" s="16"/>
     </row>
     <row r="205" ht="15.75" customHeight="1">
-      <c r="C205" s="14"/>
+      <c r="C205" s="16"/>
     </row>
     <row r="206" ht="15.75" customHeight="1">
-      <c r="C206" s="14"/>
+      <c r="C206" s="16"/>
     </row>
     <row r="207" ht="15.75" customHeight="1">
-      <c r="C207" s="14"/>
+      <c r="C207" s="16"/>
     </row>
     <row r="208" ht="15.75" customHeight="1">
-      <c r="C208" s="14"/>
+      <c r="C208" s="16"/>
     </row>
     <row r="209" ht="15.75" customHeight="1">
-      <c r="C209" s="14"/>
+      <c r="C209" s="16"/>
     </row>
     <row r="210" ht="15.75" customHeight="1">
-      <c r="C210" s="14"/>
+      <c r="C210" s="16"/>
     </row>
     <row r="211" ht="15.75" customHeight="1">
-      <c r="C211" s="14"/>
+      <c r="C211" s="16"/>
     </row>
     <row r="212" ht="15.75" customHeight="1">
-      <c r="C212" s="14"/>
+      <c r="C212" s="16"/>
     </row>
     <row r="213" ht="15.75" customHeight="1">
-      <c r="C213" s="14"/>
+      <c r="C213" s="16"/>
     </row>
     <row r="214" ht="15.75" customHeight="1">
-      <c r="C214" s="14"/>
+      <c r="C214" s="16"/>
     </row>
     <row r="215" ht="15.75" customHeight="1">
-      <c r="C215" s="14"/>
+      <c r="C215" s="16"/>
     </row>
     <row r="216" ht="15.75" customHeight="1">
-      <c r="C216" s="14"/>
+      <c r="C216" s="16"/>
     </row>
     <row r="217" ht="15.75" customHeight="1">
-      <c r="C217" s="14"/>
+      <c r="C217" s="16"/>
     </row>
     <row r="218" ht="15.75" customHeight="1">
-      <c r="C218" s="14"/>
+      <c r="C218" s="16"/>
     </row>
     <row r="219" ht="15.75" customHeight="1">
-      <c r="C219" s="14"/>
+      <c r="C219" s="16"/>
     </row>
     <row r="220" ht="15.75" customHeight="1">
-      <c r="C220" s="14"/>
+      <c r="C220" s="16"/>
     </row>
     <row r="221" ht="15.75" customHeight="1"/>
     <row r="222" ht="15.75" customHeight="1"/>

</xml_diff>